<commit_message>
- Create inner _delete_serialized_records since it is relevant for FRA now too - Dup manager now sends all fields to error generator - Add DuplicateManager as member to FRA parser - Move hash functions to base RowSchema - Update FRA row schema to generate all cat4 errors - Update test_parse_fra_ofa_test_cases to test records are removed if serialized when case has cat4 error. Also accounts for duplicate checks - Updated test files to include more dup cases
</commit_message>
<xml_diff>
--- a/tdrs-backend/tdpservice/parsers/test/data/fra_ofa_test.xlsx
+++ b/tdrs-backend/tdpservice/parsers/test/data/fra_ofa_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hhsgov-my.sharepoint.com/personal/alexandra_pennington_acf_hhs_gov/Documents/HomeDrive/win11upgrade/dummydata/qasp/FRA_WOTE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlipe/work/repos/tdrs/TANF-app/tdrs-backend/tdpservice/parsers/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{831E0306-6755-4940-B19E-02CEB9752F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACFF8AA-2566-7F4C-9D44-9A547C5CF3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="5730" windowWidth="30465" windowHeight="13620"/>
+    <workbookView xWindow="40020" yWindow="5740" windowWidth="40000" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_XLSX" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,9 +585,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -625,7 +625,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -731,7 +731,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -873,23 +873,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>202504</v>
       </c>
@@ -897,7 +897,7 @@
         <v>912345678</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>202504</v>
       </c>
@@ -905,7 +905,7 @@
         <v>987654321</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>202505</v>
       </c>
@@ -913,7 +913,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>202506</v>
       </c>
@@ -921,7 +921,7 @@
         <v>900012345</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>202505</v>
       </c>
@@ -929,7 +929,7 @@
         <v>912300012</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>202504</v>
       </c>
@@ -937,7 +937,7 @@
         <v>911222333</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>202506</v>
       </c>
@@ -945,7 +945,7 @@
         <v>912345678</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>202505</v>
       </c>
@@ -953,7 +953,7 @@
         <v>900000000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>202504</v>
       </c>
@@ -961,7 +961,7 @@
         <v>912345678</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>202506</v>
       </c>
@@ -969,7 +969,7 @@
         <v>912233445</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>202505</v>
       </c>
@@ -977,7 +977,7 @@
         <v>933344555</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>202506</v>
       </c>
@@ -985,7 +985,7 @@
         <v>944455566</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>202504</v>
       </c>
@@ -993,7 +993,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>202505</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>202604</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>202594</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>202408</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>999000999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>202506</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>202510</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>955566677</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>203001</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>988899911</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>202407</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>202411</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>979846513</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>202402</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>912345678</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>202406</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>202504</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>202594</v>
       </c>
@@ -1097,12 +1097,20 @@
         <v>91234567890</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>202508</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>202504</v>
+      </c>
+      <c r="B28">
+        <v>912345678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Update TE1 dup detector to ignore records with SSN === all 9's - Added test case to test files
</commit_message>
<xml_diff>
--- a/tdrs-backend/tdpservice/parsers/test/data/fra_ofa_test.xlsx
+++ b/tdrs-backend/tdpservice/parsers/test/data/fra_ofa_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlipe/work/repos/tdrs/TANF-app/tdrs-backend/tdpservice/parsers/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACFF8AA-2566-7F4C-9D44-9A547C5CF3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E77B423-3395-4D46-B1BB-548393715529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="5740" windowWidth="40000" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38900" yWindow="4940" windowWidth="40000" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_XLSX" sheetId="1" r:id="rId1"/>
@@ -884,10 +884,13 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B28"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
@@ -987,7 +990,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>202504</v>
+        <v>202505</v>
       </c>
       <c r="B13">
         <v>999999999</v>

</xml_diff>